<commit_message>
Teste do xlsx txt
</commit_message>
<xml_diff>
--- a/monografia/Planilha_de_Custos.xlsx
+++ b/monografia/Planilha_de_Custos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC\SMG\Monografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAB0367-BADA-4D1F-B542-ADE26785E562}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E14A0-0E77-4788-8E14-E54FFB79CF6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28455" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0ACE1672-DD9A-4472-9C4C-6E14B9B1198E}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,14 +887,14 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
         <v>0.2</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D54" s="2">
         <f>SUM(D4:D53)</f>
-        <v>186.84000000000003</v>
+        <v>186.64000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
teste depois de reiniciar
</commit_message>
<xml_diff>
--- a/monografia/Planilha_de_Custos.xlsx
+++ b/monografia/Planilha_de_Custos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC\SMG\Monografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ACBA99-8BD0-41C3-B658-C8E0996F57AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BB7CA0-0EC5-40B3-943C-0CCAF7BE6BCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28455" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0ACE1672-DD9A-4472-9C4C-6E14B9B1198E}"/>
   </bookViews>
@@ -491,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4948BA0-E1AC-4AAF-9C86-AE9BF8125C9B}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -887,14 +887,14 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="1">
         <v>0.2</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D54" s="2">
         <f>SUM(D4:D53)</f>
-        <v>186.64000000000001</v>
+        <v>186.84000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrigida valor da planilha de custo
</commit_message>
<xml_diff>
--- a/monografia/Planilha_de_Custos.xlsx
+++ b/monografia/Planilha_de_Custos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCC\SMG\Monografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BB7CA0-0EC5-40B3-943C-0CCAF7BE6BCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D982BB4-E653-4397-BBE4-E34B1C80D7AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28455" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0ACE1672-DD9A-4472-9C4C-6E14B9B1198E}"/>
   </bookViews>
@@ -887,14 +887,14 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
         <v>0.2</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D54" s="2">
         <f>SUM(D4:D53)</f>
-        <v>186.84000000000003</v>
+        <v>186.64000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>